<commit_message>
added bootmode and bootloader. disable port control.
</commit_message>
<xml_diff>
--- a/m1eph.xlsx
+++ b/m1eph.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tranka/Documents/SPI-slave/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tranka/Documents/m1_eph_fw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CA45C4-3151-7A49-B6C4-D1B5354F6054}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAC908E-B85A-A748-80C6-225632B9720D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" xr2:uid="{9F87A2BB-F86C-7C43-A7C6-278DB81C484C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="182">
   <si>
     <t>Device Profile:</t>
   </si>
@@ -679,6 +679,15 @@
   </si>
   <si>
     <t>msthb</t>
+  </si>
+  <si>
+    <t>0x8005</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>Unique_id</t>
   </si>
 </sst>
 </file>
@@ -1120,10 +1129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2EEA3DD-8C8D-5945-A9AC-0723D8A7F05C}">
-  <dimension ref="B1:T210"/>
+  <dimension ref="B1:T213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="N199" sqref="N199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -4806,55 +4815,37 @@
         <v>41</v>
       </c>
     </row>
-    <row r="201" spans="2:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B201" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C201" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D201" s="10"/>
-      <c r="E201" s="10"/>
-      <c r="F201" s="10"/>
-      <c r="G201" s="10"/>
-      <c r="H201" s="10"/>
-      <c r="I201" s="10"/>
-      <c r="J201" s="10"/>
-      <c r="K201" s="10"/>
-      <c r="L201" s="10"/>
-      <c r="M201" s="10"/>
-      <c r="N201" s="10"/>
-      <c r="O201" s="10"/>
-      <c r="P201" s="10"/>
+    <row r="201" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B201" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F201" s="1" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="202" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D202" s="13"/>
-      <c r="E202" s="9"/>
-      <c r="F202" s="9"/>
-      <c r="G202" s="9"/>
-      <c r="H202" s="9"/>
-      <c r="I202" s="9"/>
-      <c r="N202"/>
-      <c r="O202"/>
-      <c r="P202"/>
-    </row>
-    <row r="203" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D203" s="13"/>
-      <c r="E203" s="9"/>
-      <c r="F203" s="9"/>
-      <c r="G203" s="9"/>
-      <c r="H203" s="9"/>
-      <c r="I203" s="9"/>
-      <c r="N203"/>
-      <c r="O203"/>
-      <c r="P203"/>
+      <c r="D202" s="1">
+        <v>1</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="L202" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="204" spans="2:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B204" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C204" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D204" s="10"/>
       <c r="E204" s="10"/>
@@ -4892,105 +4883,148 @@
       <c r="O206"/>
       <c r="P206"/>
     </row>
-    <row r="207" spans="2:16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B207" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C207" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D207" s="15"/>
-      <c r="E207" s="15"/>
-      <c r="F207" s="15"/>
-      <c r="G207" s="15"/>
-      <c r="H207" s="15"/>
-      <c r="I207" s="15"/>
-      <c r="J207" s="15"/>
-      <c r="K207" s="15"/>
-      <c r="L207" s="15"/>
-      <c r="M207" s="15"/>
-      <c r="N207" s="15"/>
+    <row r="207" spans="2:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B207" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C207" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D207" s="10"/>
+      <c r="E207" s="10"/>
+      <c r="F207" s="10"/>
+      <c r="G207" s="10"/>
+      <c r="H207" s="10"/>
+      <c r="I207" s="10"/>
+      <c r="J207" s="10"/>
+      <c r="K207" s="10"/>
+      <c r="L207" s="10"/>
+      <c r="M207" s="10"/>
+      <c r="N207" s="10"/>
       <c r="O207" s="10"/>
       <c r="P207" s="10"/>
     </row>
     <row r="208" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B208" t="s">
-        <v>72</v>
-      </c>
-      <c r="C208" t="s">
-        <v>40</v>
-      </c>
-      <c r="D208"/>
-      <c r="E208"/>
-      <c r="F208" t="s">
-        <v>1</v>
-      </c>
-      <c r="G208"/>
-      <c r="H208"/>
-      <c r="I208"/>
-      <c r="J208" t="s">
-        <v>73</v>
-      </c>
-      <c r="K208"/>
-      <c r="L208"/>
-      <c r="M208"/>
+      <c r="D208" s="13"/>
+      <c r="E208" s="9"/>
+      <c r="F208" s="9"/>
+      <c r="G208" s="9"/>
+      <c r="H208" s="9"/>
+      <c r="I208" s="9"/>
       <c r="N208"/>
       <c r="O208"/>
       <c r="P208"/>
     </row>
     <row r="209" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B209"/>
-      <c r="C209"/>
-      <c r="D209">
-        <v>1</v>
-      </c>
-      <c r="E209" t="s">
-        <v>57</v>
-      </c>
-      <c r="F209" t="s">
-        <v>74</v>
-      </c>
-      <c r="G209" t="s">
-        <v>75</v>
-      </c>
-      <c r="H209"/>
-      <c r="I209"/>
-      <c r="J209" t="s">
-        <v>73</v>
-      </c>
-      <c r="K209"/>
-      <c r="L209" t="s">
-        <v>41</v>
-      </c>
-      <c r="M209"/>
-      <c r="N209" s="16"/>
+      <c r="D209" s="13"/>
+      <c r="E209" s="9"/>
+      <c r="F209" s="9"/>
+      <c r="G209" s="9"/>
+      <c r="H209" s="9"/>
+      <c r="I209" s="9"/>
+      <c r="N209"/>
       <c r="O209"/>
       <c r="P209"/>
     </row>
-    <row r="210" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B210"/>
-      <c r="C210"/>
-      <c r="D210">
+    <row r="210" spans="2:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B210" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C210" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D210" s="15"/>
+      <c r="E210" s="15"/>
+      <c r="F210" s="15"/>
+      <c r="G210" s="15"/>
+      <c r="H210" s="15"/>
+      <c r="I210" s="15"/>
+      <c r="J210" s="15"/>
+      <c r="K210" s="15"/>
+      <c r="L210" s="15"/>
+      <c r="M210" s="15"/>
+      <c r="N210" s="15"/>
+      <c r="O210" s="10"/>
+      <c r="P210" s="10"/>
+    </row>
+    <row r="211" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B211" t="s">
+        <v>72</v>
+      </c>
+      <c r="C211" t="s">
+        <v>40</v>
+      </c>
+      <c r="D211"/>
+      <c r="E211"/>
+      <c r="F211" t="s">
+        <v>1</v>
+      </c>
+      <c r="G211"/>
+      <c r="H211"/>
+      <c r="I211"/>
+      <c r="J211" t="s">
+        <v>73</v>
+      </c>
+      <c r="K211"/>
+      <c r="L211"/>
+      <c r="M211"/>
+      <c r="N211"/>
+      <c r="O211"/>
+      <c r="P211"/>
+    </row>
+    <row r="212" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B212"/>
+      <c r="C212"/>
+      <c r="D212">
+        <v>1</v>
+      </c>
+      <c r="E212" t="s">
+        <v>57</v>
+      </c>
+      <c r="F212" t="s">
+        <v>74</v>
+      </c>
+      <c r="G212" t="s">
+        <v>75</v>
+      </c>
+      <c r="H212"/>
+      <c r="I212"/>
+      <c r="J212" t="s">
+        <v>73</v>
+      </c>
+      <c r="K212"/>
+      <c r="L212" t="s">
+        <v>41</v>
+      </c>
+      <c r="M212"/>
+      <c r="N212" s="16"/>
+      <c r="O212"/>
+      <c r="P212"/>
+    </row>
+    <row r="213" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B213"/>
+      <c r="C213"/>
+      <c r="D213">
         <v>2</v>
       </c>
-      <c r="E210" t="s">
+      <c r="E213" t="s">
         <v>57</v>
       </c>
-      <c r="F210" t="s">
+      <c r="F213" t="s">
         <v>76</v>
       </c>
-      <c r="G210"/>
-      <c r="H210"/>
-      <c r="I210"/>
-      <c r="J210" t="s">
+      <c r="G213"/>
+      <c r="H213"/>
+      <c r="I213"/>
+      <c r="J213" t="s">
         <v>73</v>
       </c>
-      <c r="K210"/>
-      <c r="L210" t="s">
-        <v>41</v>
-      </c>
-      <c r="M210"/>
-      <c r="N210"/>
+      <c r="K213"/>
+      <c r="L213" t="s">
+        <v>41</v>
+      </c>
+      <c r="M213"/>
+      <c r="N213"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4998,20 +5032,20 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Backup/Setting Flag" error="The entry flag shall be_x000a_B : (Backup)_x000a_S : (Setting)" sqref="K12:K13 K15:K16 K18:K19 K21:K22 K27:K28 K30:K31 K33:K34 K24:K25 K36:K39 K202:K203 K205:K210 K133:K200 K77:K92 K95:K131" xr:uid="{1A6CC9A1-B41D-2E4A-B18E-EEC18736D512}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Backup/Setting Flag" error="The entry flag shall be_x000a_B : (Backup)_x000a_S : (Setting)" sqref="K12:K13 K15:K16 K18:K19 K21:K22 K27:K28 K30:K31 K33:K34 K24:K25 K36:K39 K205:K206 K208:K213 K133:K203 K77:K92 K95:K131" xr:uid="{1A6CC9A1-B41D-2E4A-B18E-EEC18736D512}">
       <formula1>"B,S"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Category" error="The value for the entry category shall be _x000a_M : (mandatory)_x000a_O : (optional) _x000a_C : (conditional)" sqref="J12:J13 J15:J16 J18:J19 J21:J22 J27:J28 J30:J31 J33:J34 J24:J25 J36:J39 J202:J203 J205:J210 J133:J200 J77:J92 J95:J131" xr:uid="{19E02EBF-1A37-B34F-951C-1141CF0F2A70}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Category" error="The value for the entry category shall be _x000a_M : (mandatory)_x000a_O : (optional) _x000a_C : (conditional)" sqref="J12:J13 J15:J16 J18:J19 J21:J22 J27:J28 J30:J31 J33:J34 J24:J25 J36:J39 J205:J206 J208:J213 J133:J203 J77:J92 J95:J131" xr:uid="{19E02EBF-1A37-B34F-951C-1141CF0F2A70}">
       <formula1>"M,O,C"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="C11 C14 C17 C20 C23 C26 C29 C32 C35 C94 C132 C201 C204" xr:uid="{A4BD42A4-2ED5-AC4A-8771-5F5AD36F2FEC}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Object Code value" error="The Object code value shall be:_x000a_VARIABLE_x000a_RECORD_x000a_ARRAY" sqref="C12:C13 C15:C16 C18:C19 C21:C22 C27:C28 C30:C31 C33:C34 C24:C25 C36:C39 C202:C203 C205:C210 C133:C200 C77:C92 C95:C131" xr:uid="{A8951C0B-BE51-E340-ABAE-83CEB5BD45B8}">
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="C11 C14 C17 C20 C23 C26 C29 C32 C35 C94 C132 C204 C207" xr:uid="{A4BD42A4-2ED5-AC4A-8771-5F5AD36F2FEC}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Object Code value" error="The Object code value shall be:_x000a_VARIABLE_x000a_RECORD_x000a_ARRAY" sqref="C12:C13 C15:C16 C18:C19 C21:C22 C27:C28 C30:C31 C33:C34 C24:C25 C36:C39 C205:C206 C208:C213 C133:C203 C77:C92 C95:C131" xr:uid="{A8951C0B-BE51-E340-ABAE-83CEB5BD45B8}">
       <formula1>"VARIABLE,ARRAY,RECORD"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M15:M16 M18:M19 M21:M22 M27:M28 M30:M31 M33:M34 M24:M25 M12:M13 M36:M39 M202:M203 M205:M208 M133:M200 M45:M93 M95:M131" xr:uid="{02EEC6B4-E903-9C4A-A638-20D4927F3E8B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M15:M16 M18:M19 M21:M22 M27:M28 M30:M31 M33:M34 M24:M25 M12:M13 M36:M39 M205:M206 M208:M211 M133:M203 M45:M93 M95:M131" xr:uid="{02EEC6B4-E903-9C4A-A638-20D4927F3E8B}">
       <formula1>"rx,tx"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C211:C1049" xr:uid="{C233EF9B-F7E6-A740-A411-47093AA361DC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C214:C1052" xr:uid="{C233EF9B-F7E6-A740-A411-47093AA361DC}">
       <formula1>"VARIABLE,ARRAY,RECORD"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>